<commit_message>
Added the test value key for the AES example
</commit_message>
<xml_diff>
--- a/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
+++ b/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88215cb98efcb80/Documents/Excel experiments/ExcelExampleAndMakroSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{87CA9812-2E90-4477-BC68-45A1574C2952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D186C6B9-4647-4C5F-B53B-757E33145AFC}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{18DE7318-FF27-42B6-86B1-636905DBE40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CDD3D6-9F2A-4538-B52B-9E8CBDA4734C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="571">
   <si>
     <t>Plain</t>
   </si>
@@ -2411,7 +2411,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2492,9 +2492,8 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="C17">
-        <f>F17</f>
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3">

</xml_diff>

<commit_message>
Added taglen as argument for openssl_aesgcm.c as well as on the Excel side AES_Encrypt
</commit_message>
<xml_diff>
--- a/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
+++ b/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88215cb98efcb80/Documents/Excel experiments/ExcelExampleAndMakroSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{18DE7318-FF27-42B6-86B1-636905DBE40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CDD3D6-9F2A-4538-B52B-9E8CBDA4734C}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D495C800-C295-49CE-B013-35DFA772AE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50037885-D4B8-4AA1-A789-410D2C790364}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="576">
   <si>
     <t>Plain</t>
   </si>
@@ -1169,9 +1169,6 @@
   </si>
   <si>
     <t>Public Function Util_GenRandom(ByVal size As Long) As String</t>
-  </si>
-  <si>
-    <t>Public Function AES_Encrypt(ByVal key As String, ByVal plain As String, Optional ByVal mode As String = "CBC", Optional ByVal iv As String = "") As String</t>
   </si>
   <si>
     <t>Public Function AES_Decrypt(ByVal key As String, ByVal cipher As String, Optional ByVal mode As String = "CBC", Optional ByVal iv As String = "", Optional ByVal GCMtagLen As Long = 12) As String</t>
@@ -1708,18 +1705,6 @@
   </si>
   <si>
     <t>------------------------------------------------------------------------------------------------------_x000D_
-' AES_Encrypt (key, plain, mode, iv) encrypts plain with AES algorithm_x000D_
-' key           : The AES key in hex string_x000D_
-' plain         : A hex string with the plain data to be encrypted_x000D_
-' mode          : If ECB or CBC encryption will be done with chaining mode ECB/CBC and PKCS7 padding_x000D_
-'                 if mode=GCM then encryption will be done following the GCM pattern_x000D_
-'                 in that case the resulting TAG willl be appended to the resulting cipher text_x000D_
-'                 at present only default taglen (12) - implemented TBD_x000D_
-' IV            : IV hex string with initialization vector should be 16 for ECB &amp; CBC 12 for GCM_x000D_
-'-------------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>------------------------------------------------------------------------------------------------------_x000D_
 ' AES_Decrypt (key, cipher, mode, iv, gcmTagLen) decrypts cipher with AES algorithm_x000D_
 ' key           : The AES key in hex string_x000D_
 ' cipher        : Hes string wiht the cipher text_x000D_
@@ -1981,6 +1966,37 @@
   </si>
   <si>
     <t>Alice &amp; Bob's keys are includign in the Keys worksheet as well as in the openssl directories.</t>
+  </si>
+  <si>
+    <t>486920416C69636520776861742061626F75742064696E6E657220746F6E69676874203F</t>
+  </si>
+  <si>
+    <t>IV - Nonce 12 bytes</t>
+  </si>
+  <si>
+    <t>TagLen</t>
+  </si>
+  <si>
+    <t>8914fdf7b77a70a521931ba7994a306d629db66863c063077c6e8f5381fe9434</t>
+  </si>
+  <si>
+    <t>07e07d3ac1aaedf2fdfe5a4e</t>
+  </si>
+  <si>
+    <t>------------------------------------------------------------------------------------------------------_x000D_
+' AES_Encrypt (key, plain, mode, iv) encrypts plain with AES algorithm_x000D_
+' key           : The AES key in hex string_x000D_
+' plain         : A hex string with the plain data to be encrypted_x000D_
+' mode          : If ECB or CBC encryption will be done with chaining mode ECB/CBC and PKCS7 padding_x000D_
+'                 if mode=GCM then encryption will be done following the GCM pattern_x000D_
+'                 in that case the resulting TAG willl be appended to the resulting cipher text_x000D_
+'                 at present only default taglen (12) - implemented TBD_x000D_
+' IV            : IV hex string with initialization vector should be 16 for ECB &amp; CBC 12 for GCM_x000D_
+' GCMtagLen     : The length of the TAG expected to be a the end of the string (OBS only 12 tested)_x000D_
+'-------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Public Function AES_Encrypt(ByVal key As String, ByVal plain As String, Optional ByVal mode As String = "CBC", Optional ByVal iv As String = "", Optional ByVal GCMtagLen As Long = 12) As String</t>
   </si>
 </sst>
 </file>
@@ -2422,70 +2438,70 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="20" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="20" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2498,7 +2514,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B18" t="str" cm="1">
         <f t="array" ref="B18">Util_showFormula(C18)</f>
@@ -2519,7 +2535,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C20" t="str">
         <f>"01020304050607080102030405060708"</f>
@@ -2528,38 +2544,38 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C21" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="20" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -3721,10 +3737,10 @@
         <v>96</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="108.6">
@@ -3732,21 +3748,21 @@
         <v>97</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>500</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="96.6">
       <c r="A3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>502</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="84.6">
@@ -3754,18 +3770,18 @@
         <v>291</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>504</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120.6">
       <c r="A5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>357</v>
@@ -3773,10 +3789,10 @@
     </row>
     <row r="6" spans="1:3" ht="108.6">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>358</v>
@@ -3784,10 +3800,10 @@
     </row>
     <row r="7" spans="1:3" ht="84.6">
       <c r="A7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>359</v>
@@ -3795,46 +3811,46 @@
     </row>
     <row r="8" spans="1:3" ht="168.6">
       <c r="A8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>509</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="96.6">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="120.6">
       <c r="A10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="96.6">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>513</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="84.6">
@@ -3842,7 +3858,7 @@
         <v>219</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>360</v>
@@ -3853,7 +3869,7 @@
         <v>230</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>361</v>
@@ -3861,35 +3877,35 @@
     </row>
     <row r="14" spans="1:3" ht="84.6">
       <c r="A14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="144.6">
+    <row r="15" spans="1:3" ht="156.6">
       <c r="A15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>518</v>
+        <v>574</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>367</v>
+        <v>575</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="156.6">
       <c r="A16" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="108.6">
@@ -3897,10 +3913,10 @@
         <v>232</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="108.6">
@@ -3908,128 +3924,128 @@
         <v>233</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="96.6">
       <c r="A19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="96.6">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="96.6">
       <c r="A21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="84.6">
       <c r="A22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="72.599999999999994">
       <c r="A23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="72.599999999999994">
       <c r="A24" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="84.6">
       <c r="A25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="84.6">
       <c r="A26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="84.6">
       <c r="A27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="84.6">
       <c r="A28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="72.599999999999994">
       <c r="A29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>366</v>
@@ -4037,21 +4053,21 @@
     </row>
     <row r="30" spans="1:3" ht="72.599999999999994">
       <c r="A30" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="72.599999999999994">
       <c r="A31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>362</v>
@@ -4059,10 +4075,10 @@
     </row>
     <row r="32" spans="1:3" ht="72.599999999999994">
       <c r="A32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>363</v>
@@ -4070,21 +4086,21 @@
     </row>
     <row r="33" spans="1:3" ht="72.599999999999994">
       <c r="A33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="72.599999999999994">
       <c r="A34" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>364</v>
@@ -4092,68 +4108,68 @@
     </row>
     <row r="35" spans="1:3" ht="84.6">
       <c r="A35" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="84.6">
       <c r="A36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="108.6">
       <c r="A37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="108.6">
       <c r="A38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="96.6">
       <c r="A39" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="72.599999999999994">
       <c r="A40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -4244,7 +4260,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">Util_GenRandom(32)</f>
-        <v>1988719BCEB0C3302E3AF7D2920B87B7AD65BFA240D1960237C3965D74EFEB29</v>
+        <v>E62B9DE0FBFD8C9D80E010B4742C370262A75131C8FB2A40AE1A18EB3C41AE58</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4262,7 +4278,7 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">Util_GenRandom((16))</f>
-        <v>4CA16B8EC2BF9A950388106B8522397E</v>
+        <v>169F6AA1D13E75824C3B1FBB06F3F8D7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4275,7 +4291,7 @@
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">Util_HexStrToBase64(C9)</f>
-        <v>TKFrjsK/mpUDiBBrhSI5fg==</v>
+        <v>Fp9qodE+dYJMOx+7BvP41w==</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4322,7 +4338,7 @@
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">AES_Encrypt(C7,C13,C14,C9)</f>
-        <v>8FA9D4CD577074AC06A9C92EA53D586D4E828E32AD08E841DF8B9034E4278B729A00EB5DD8D21B96D01648221343838A</v>
+        <v>BBA8318AC4F3ECBF823680F681F14CF8BE7A4661F02C5FA7E2F2A47052B05B90822EF3EA0F9C0A24464AAE9031C4B982</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4335,7 +4351,7 @@
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">Util_HexStrToBase64(C16)</f>
-        <v>j6nUzVdwdKwGqckupT1YbU6CjjKtCOhB34uQNOQni3KaAOtd2NIbltAWSCITQ4OK</v>
+        <v>u6gxisTz7L+CNoD2gfFM+L56RmHwLF+n4vKkcFKwW5CCLvPqD5wKJEZKrpAxxLmC</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4449,7 +4465,7 @@
       </c>
       <c r="C31" t="str" cm="1">
         <f t="array" ref="C31">RSA_Encrypt(C29,C7,C30)</f>
-        <v>4B8A6CCBB19A0FB42D38BAC0C8F12B7DFD2AEDF99A1CFDC62349AEAE5CD45C946CE5141E59A98342F9728780C644DE7BCB20C91C7394EA878D62B6C03EBB11EB186DE627FF3E806A00AD96E5DCAF32A23F81ECBE6EE55134FFA9ED0EA7DB981827CEC5CF25FE072604186ECC79CC71C181C14753AC38D133BC1722DD3E4E6A8503695365E413E0B0120764B49176611F5C7DC5849B8C15C2015A07C463B2B82F4939FB5741CFCCE5A20B83C1610801042E1FBF35D339B603922EBD31642177F3E01E325C236E56A0EBACADF2623E0F28ACCCB004A376E24F535DF37926051E6709F4FB1C34D9BB2A8C427A8E4EA3E59AC093198FFD7DB0FD046E63079F274FF6</v>
+        <v>6C3822787D0389B2E080927048283B81C31121A4F18BBE50C5532D9F6033B3F56FCCFDC678DC977C5896AC7C200C6A0116B347E8526B0378B824DEE43DBE2D659CE85FB5B3D9EBB4D69CE8040B7F81EBED9B7F73E1A0BBC3A556DA45CF83C47D1B49BFFF24B6880782D28384BB6AD9C22D61E65B0F6DD73F24F1965920BFA89D5A24A38EA1A1C479B3E4EDE326AE420E6C191E1E1D18906958A032C7140B05F2DB3468063704143A5FB842E6A31FFC2DDDC5A3D18CE89A3681256A0F75F9804A0E8B484DA061DF4536748A50E87258270A9C41C2EAE11F196C7FD4308B01DBDD177AD822FDB798C83F5A8C697399B0CFF9987AF0E5E351FBDB5B191118533C26</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4462,12 +4478,12 @@
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">Util_HexStrToBase64(C31)</f>
-        <v>S4psy7GaD7QtOLrAyPErff0q7fmaHP3GI0murlzUXJRs5RQeWamDQvlyh4DGRN57_x000D_
-yyDJHHOU6oeNYrbAPrsR6xht5if/PoBqAK2W5dyvMqI/gey+buVRNP+p7Q6n25gY_x000D_
-J87FzyX+ByYEGG7MecxxwYHBR1OsONEzvBci3T5OaoUDaVNl5BPgsBIHZLSRdmEf_x000D_
-XH3FhJuMFcIBWgfEY7K4L0k5+1dBz8zloguDwWEIAQQuH7810zm2A5IuvTFkIXfz_x000D_
-4B4yXCNuVqDrrK3yYj4PKKzMsASjduJPU13zeSYFHmcJ9PscNNm7KoxCeo5Oo+Wa_x000D_
-wJMZj/19sP0EbmMHnydP9g==</v>
+        <v>bDgieH0DibLggJJwSCg7gcMRIaTxi75QxVMtn2Azs/VvzP3GeNyXfFiWrHwgDGoB_x000D_
+FrNH6FJrA3i4JN7kPb4tZZzoX7Wz2eu01pzoBAt/gevtm39z4aC7w6VW2kXPg8R9_x000D_
+G0m//yS2iAeC0oOEu2rZwi1h5lsPbdc/JPGWWSC/qJ1aJKOOoaHEebPk7eMmrkIO_x000D_
+bBkeHh0YkGlYoDLHFAsF8ts0aAY3BBQ6X7hC5qMf/C3dxaPRjOiaNoElag91+YBK_x000D_
+DotITaBh30U2dIpQ6HJYJwqcQcLq4R8ZbH/UMIsB290Xetgi/beYyD9ajGlzmbDP_x000D_
++Zh68OXjUfvbWxkRGFM8Jg==</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4486,7 +4502,7 @@
       </c>
       <c r="C35" t="str">
         <f>C10</f>
-        <v>TKFrjsK/mpUDiBBrhSI5fg==</v>
+        <v>Fp9qodE+dYJMOx+7BvP41w==</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4500,7 +4516,7 @@
       </c>
       <c r="C36" t="str">
         <f>C17</f>
-        <v>j6nUzVdwdKwGqckupT1YbU6CjjKtCOhB34uQNOQni3KaAOtd2NIbltAWSCITQ4OK</v>
+        <v>u6gxisTz7L+CNoD2gfFM+L56RmHwLF+n4vKkcFKwW5CCLvPqD5wKJEZKrpAxxLmC</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4514,12 +4530,12 @@
       </c>
       <c r="C37" t="str">
         <f>C32</f>
-        <v>S4psy7GaD7QtOLrAyPErff0q7fmaHP3GI0murlzUXJRs5RQeWamDQvlyh4DGRN57_x000D_
-yyDJHHOU6oeNYrbAPrsR6xht5if/PoBqAK2W5dyvMqI/gey+buVRNP+p7Q6n25gY_x000D_
-J87FzyX+ByYEGG7MecxxwYHBR1OsONEzvBci3T5OaoUDaVNl5BPgsBIHZLSRdmEf_x000D_
-XH3FhJuMFcIBWgfEY7K4L0k5+1dBz8zloguDwWEIAQQuH7810zm2A5IuvTFkIXfz_x000D_
-4B4yXCNuVqDrrK3yYj4PKKzMsASjduJPU13zeSYFHmcJ9PscNNm7KoxCeo5Oo+Wa_x000D_
-wJMZj/19sP0EbmMHnydP9g==</v>
+        <v>bDgieH0DibLggJJwSCg7gcMRIaTxi75QxVMtn2Azs/VvzP3GeNyXfFiWrHwgDGoB_x000D_
+FrNH6FJrA3i4JN7kPb4tZZzoX7Wz2eu01pzoBAt/gevtm39z4aC7w6VW2kXPg8R9_x000D_
+G0m//yS2iAeC0oOEu2rZwi1h5lsPbdc/JPGWWSC/qJ1aJKOOoaHEebPk7eMmrkIO_x000D_
+bBkeHh0YkGlYoDLHFAsF8ts0aAY3BBQ6X7hC5qMf/C3dxaPRjOiaNoElag91+YBK_x000D_
+DotITaBh30U2dIpQ6HJYJwqcQcLq4R8ZbH/UMIsB290Xetgi/beYyD9ajGlzmbDP_x000D_
++Zh68OXjUfvbWxkRGFM8Jg==</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -4789,7 +4805,7 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A7" sqref="A7:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4845,7 +4861,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">Util_GenRandom(32)</f>
-        <v>662CB3A35E6B27B377F46EC82CA4608C0C3C67C41CFB5F13AF46DE96726E29D1</v>
+        <v>A6893B147B859F4865A4F9688361DFD7750E1D2FC31BF9A61995D6DFF9342639</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4863,7 +4879,7 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">Util_GenRandom((12))</f>
-        <v>5792435BF272944E992B9F2E</v>
+        <v>319012BC1DA1734ACB44E881</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4876,7 +4892,7 @@
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">Util_HexStrToBase64(C9)</f>
-        <v>V5JDW/JylE6ZK58u</v>
+        <v>MZASvB2hc0rLROiB</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4923,7 +4939,7 @@
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">AES_Encrypt(C7,C13,C14,C9)</f>
-        <v>754D94FC5A6920EA7E1FF06C5CAD868566BE38C95DFBCBA07FD860948DDB03C3742887B5802223AD1A889661DB409EDF</v>
+        <v>9E6480D973EBFCA33F35D717B1B99DAEA3A40C49DC9823A4050C5FD1843890319898ED5810414162EBFC6C1EB29E1386</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4941,7 +4957,7 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">Util_HexStrToBase64(C16)</f>
-        <v>dU2U/FppIOp+H/BsXK2GhWa+OMld+8ugf9hglI3bA8N0KIe1gCIjrRqIlmHbQJ7f</v>
+        <v>nmSA2XPr/KM/NdcXsbmdrqOkDEncmCOkBQxf0YQ4kDGYmO1YEEFBYuv8bB6ynhOG</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4956,7 +4972,7 @@
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">GCM_getEncrypted(C16)</f>
-        <v>754D94FC5A6920EA7E1FF06C5CAD868566BE38C95DFBCBA07FD860948DDB03C3742887B5</v>
+        <v>9E6480D973EBFCA33F35D717B1B99DAEA3A40C49DC9823A4050C5FD1843890319898ED58</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4966,7 +4982,7 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">GCM_getTag(C16)</f>
-        <v>802223AD1A889661DB409EDF</v>
+        <v>10414162EBFC6C1EB29E1386</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5106,7 +5122,7 @@
       </c>
       <c r="C39" t="str" cm="1">
         <f t="array" ref="C39">RSA_Encrypt(C34,C7,C35,C36,C37)</f>
-        <v>6329ECBA2A9BC6D665EF89BA615A34145AF3DCD9FACDA753FB143EE455F1073740819EC6D56329035A4504B748438189BDD11C9D893C03557069FF794B6463761D412139BFEC790DAE1A1F874BE9F819889AB8BB4C230A82863E0D1583A76BD96B8E0E3498116471E981E2F190E934026FDF1D105CC59AED870CABDA79F6E9F2D02C738E02A24505E1D2FC8C87BF4D6272E5521EF3434FBC9F02E7C62BC65447ADD16ADE7516104B49DEABEEA77EEE16EF7BC807F393EE055CC3AED09EA112A6FC1685714A794853217DFC86F031A7F7D608CC768664A56299B0DE7D05E43012157F2E827C1FC756EB8C3A21D6AD039B19FAB46009639669BE3788B4E7B73D7C</v>
+        <v>64C0FB287838A1B0168A7AEA97E3CBB3B66AFDD5338DF02FBB497095159F4CBBBCC54575DB60027B569C4FDA5A786D23E7C37CC8124A8C40DD5DCD6270DAD5EFC7FFB8B68A9148A2E60E6F0A762ECC6EC19A4481D6FD32040FF7CB685CA07D363F240090BE21416AFABECB1B2CFBC2DE3BAF3720CFDB294DD5FEBA99F1CB101DDD47E959204B754CF46E993C3374BB91A9F15A2616407B9BB804E2ADE1B8ADC98F6F6F35DD3E4B92115CA3E9C601B373E95CD55E0D546BEDEC033DA5A6245A870EF497C303C6A1391F722F9D25D9EB63C884809FA217616B280F9ECC96D2C4BA424331E030CF12ACF3736FB5A9CD4415EFF89726D9E7DDFB7B3BD84DD0BB1A57</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5119,12 +5135,12 @@
       </c>
       <c r="C40" t="str" cm="1">
         <f t="array" ref="C40">Util_HexStrToBase64(C39)</f>
-        <v>YynsuiqbxtZl74m6YVo0FFrz3Nn6zadT+xQ+5FXxBzdAgZ7G1WMpA1pFBLdIQ4GJ_x000D_
-vdEcnYk8A1Vwaf95S2Rjdh1BITm/7HkNrhofh0vp+BmImri7TCMKgoY+DRWDp2vZ_x000D_
-a44ONJgRZHHpgeLxkOk0Am/fHRBcxZrthwyr2nn26fLQLHOOAqJFBeHS/IyHv01i_x000D_
-cuVSHvNDT7yfAufGK8ZUR63Rat51FhBLSd6r7qd+7hbve8gH85PuBVzDrtCeoRKm_x000D_
-/BaFcUp5SFMhffyG8DGn99YIzHaGZKVimbDefQXkMBIVfy6CfB/HVuuMOiHWrQOb_x000D_
-Gfq0YAljlmm+N4i057c9fA==</v>
+        <v>ZMD7KHg4obAWinrql+PLs7Zq/dUzjfAvu0lwlRWfTLu8xUV122ACe1acT9paeG0j_x000D_
+58N8yBJKjEDdXc1icNrV78f/uLaKkUii5g5vCnYuzG7BmkSB1v0yBA/3y2hcoH02_x000D_
+PyQAkL4hQWr6vssbLPvC3juvNyDP2ylN1f66mfHLEB3dR+lZIEt1TPRumTwzdLuR_x000D_
+qfFaJhZAe5u4BOKt4bityY9vbzXdPkuSEVyj6cYBs3PpXNVeDVRr7ewDPaWmJFqH_x000D_
+DvSXwwPGoTkfci+dJdnrY8iEgJ+iF2FrKA+ezJbSxLpCQzHgMM8SrPNzb7WpzUQV_x000D_
+7/iXJtnn3ft7O9hN0LsaVw==</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -5142,7 +5158,7 @@
       </c>
       <c r="C43" t="str">
         <f>C10</f>
-        <v>V5JDW/JylE6ZK58u</v>
+        <v>MZASvB2hc0rLROiB</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -5156,7 +5172,7 @@
       </c>
       <c r="C44" t="str">
         <f>C18</f>
-        <v>dU2U/FppIOp+H/BsXK2GhWa+OMld+8ugf9hglI3bA8N0KIe1gCIjrRqIlmHbQJ7f</v>
+        <v>nmSA2XPr/KM/NdcXsbmdrqOkDEncmCOkBQxf0YQ4kDGYmO1YEEFBYuv8bB6ynhOG</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -5203,12 +5219,12 @@
       </c>
       <c r="C47" t="str">
         <f>C40</f>
-        <v>YynsuiqbxtZl74m6YVo0FFrz3Nn6zadT+xQ+5FXxBzdAgZ7G1WMpA1pFBLdIQ4GJ_x000D_
-vdEcnYk8A1Vwaf95S2Rjdh1BITm/7HkNrhofh0vp+BmImri7TCMKgoY+DRWDp2vZ_x000D_
-a44ONJgRZHHpgeLxkOk0Am/fHRBcxZrthwyr2nn26fLQLHOOAqJFBeHS/IyHv01i_x000D_
-cuVSHvNDT7yfAufGK8ZUR63Rat51FhBLSd6r7qd+7hbve8gH85PuBVzDrtCeoRKm_x000D_
-/BaFcUp5SFMhffyG8DGn99YIzHaGZKVimbDefQXkMBIVfy6CfB/HVuuMOiHWrQOb_x000D_
-Gfq0YAljlmm+N4i057c9fA==</v>
+        <v>ZMD7KHg4obAWinrql+PLs7Zq/dUzjfAvu0lwlRWfTLu8xUV122ACe1acT9paeG0j_x000D_
+58N8yBJKjEDdXc1icNrV78f/uLaKkUii5g5vCnYuzG7BmkSB1v0yBA/3y2hcoH02_x000D_
+PyQAkL4hQWr6vssbLPvC3juvNyDP2ylN1f66mfHLEB3dR+lZIEt1TPRumTwzdLuR_x000D_
+qfFaJhZAe5u4BOKt4bityY9vbzXdPkuSEVyj6cYBs3PpXNVeDVRr7ewDPaWmJFqH_x000D_
+DvSXwwPGoTkfci+dJdnrY8iEgJ+iF2FrKA+ezJbSxLpCQzHgMM8SrPNzb7WpzUQV_x000D_
+7/iXJtnn3ft7O9hN0LsaVw==</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5218,7 +5234,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -5226,7 +5242,7 @@
         <v>340</v>
       </c>
       <c r="C64" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -5234,7 +5250,7 @@
         <v>341</v>
       </c>
       <c r="C65" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -5250,7 +5266,7 @@
         <v>342</v>
       </c>
       <c r="C67" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -5489,12 +5505,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I2" t="str" cm="1">
         <f t="array" ref="I2">Util_AsciiToHexStr("AliceBob")</f>
@@ -5503,7 +5519,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5534,14 +5550,14 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" ref="B7">Util_showFormula(C7)</f>
         <v>HASH</v>
       </c>
       <c r="C7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5584,7 +5600,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11">Util_showFormula(C11)</f>
@@ -5597,20 +5613,20 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" ref="B16">Util_showFormula(C16)</f>
@@ -5623,7 +5639,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B17" t="str" cm="1">
         <f t="array" ref="B17">Util_showFormula(C17)</f>
@@ -5643,12 +5659,12 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">Util_GenRandom(16)</f>
-        <v>60FEB80999524584A3FB372C79871DBB</v>
+        <v>F5F4B248D223D729A4963CEA69484697</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" ref="B19">Util_showFormula(C19)</f>
@@ -5656,12 +5672,12 @@
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">AES_Encrypt(C11,C16,C17,C18)</f>
-        <v>C307189F5BF33EF29267A55A90D8E567DE7C5094A8FD50DC6CE52A86A559BE08C2A76B6E392856C8814DEDE9CCE58D280893DC739F77744EC768AC6164E4A102</v>
+        <v>C7749A9B22A78CD40C44A1745039752BB1FBB26141609F9E1A1A3A4BDE067D69D239F80E42B4D79F38DFCCEEF1065011F57D15BAD745DB1F3BBAA1BED0D77E47</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5717,19 +5733,19 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27">Util_showFormula(C27)</f>
         <v>DER</v>
       </c>
       <c r="C27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28">Util_showFormula(C28)</f>
@@ -5737,17 +5753,17 @@
       </c>
       <c r="C28" t="str" cm="1">
         <f t="array" ref="C28">EC_SignHash(C25,C26,C27)</f>
-        <v>3044022038A1EE23AAAD227ECB031E1BA897D36F3E33B2913BC37A04541530399B3AF96702202744F118BEBD44ACD293EC4372B1F6FC3CC28F1DD19EBD3D85AF0BAB821D1450</v>
+        <v>30440220289ECCD3A98AD9C381C95225640D4F8ACB72B461ED98B40F6BAE3AC7796675A30220644EBA1ADAF12856300F6F3915122B2861DD0E80FC2254135A569DD55A556447</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B34" t="str" cm="1">
         <f t="array" ref="B34">Util_showFormula(C34)</f>
@@ -5760,7 +5776,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B35" t="str" cm="1">
         <f t="array" ref="B35">Util_showFormula(C35)</f>
@@ -5768,13 +5784,13 @@
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">Util_HexStrToBase64(C19)</f>
-        <v>wwcYn1vzPvKSZ6VakNjlZ958UJSo/VDcbOUqhqVZvgjCp2tuOShWyIFN7enM5Y0o_x000D_
-CJPcc593dE7HaKxhZOShAg==</v>
+        <v>x3SamyKnjNQMRKF0UDl1K7H7smFBYJ+eGho6S94GfWnSOfgOQrTXnzjfzO7xBlAR_x000D_
+9X0VutdF2x87uqG+0Nd+Rw==</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B36" t="str" cm="1">
         <f t="array" ref="B36">Util_showFormula(C36)</f>
@@ -5782,12 +5798,12 @@
       </c>
       <c r="C36" t="str" cm="1">
         <f t="array" ref="C36">Util_HexStrToBase64(C18)</f>
-        <v>YP64CZlSRYSj+zcseYcduw==</v>
+        <v>9fSySNIj1ymkljzqaUhGlw==</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B37" t="str" cm="1">
         <f t="array" ref="B37">Util_showFormula(C37)</f>
@@ -5795,50 +5811,50 @@
       </c>
       <c r="C37" t="str" cm="1">
         <f t="array" ref="C37">Util_HexStrToBase64(C28)</f>
-        <v>MEQCIDih7iOqrSJ+ywMeG6iX028+M7KRO8N6BFQVMDmbOvlnAiAnRPEYvr1ErNKT_x000D_
-7ENysfb8PMKPHdGevT2Frwurgh0UUA==</v>
+        <v>MEQCICiezNOpitnDgclSJWQNT4rLcrRh7Zi0D2uuOsd5ZnWjAiBkTroa2vEoVjAP_x000D_
+bzkVEisoYd0OgPwiVBNaVp3VWlVkRw==</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C43" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>454</v>
+      </c>
+      <c r="C44" t="s">
         <v>455</v>
-      </c>
-      <c r="C44" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -5869,14 +5885,14 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B50" t="str" cm="1">
         <f t="array" ref="B50">Util_showFormula(C50)</f>
         <v>HASH</v>
       </c>
       <c r="C50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -5919,7 +5935,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B54" t="str" cm="1">
         <f t="array" ref="B54">Util_showFormula(C54)</f>
@@ -5932,7 +5948,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -5950,7 +5966,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B59" t="str" cm="1">
         <f t="array" ref="B59">Util_showFormula(C59)</f>
@@ -5975,7 +5991,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B61" t="str" cm="1">
         <f t="array" ref="B61">Util_showFormula(C61)</f>
@@ -5988,7 +6004,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B62" t="str" cm="1">
         <f t="array" ref="B62">Util_showFormula(C62)</f>
@@ -6002,7 +6018,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -6071,31 +6087,31 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B71" t="str" cm="1">
         <f t="array" ref="B71">Util_showFormula(C71)</f>
         <v>DER</v>
       </c>
       <c r="C71" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B72" t="str" cm="1">
         <f t="array" ref="B72">Util_showFormula(C72)</f>
         <v>EC_VerifySignature found the mssage a being OK</v>
       </c>
       <c r="C72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B73" t="str" cm="1">
         <f t="array" ref="B73">Util_showFormula(C73)</f>
@@ -6115,10 +6131,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6478,6 +6494,87 @@
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
     </row>
+    <row r="32" spans="1:7">
+      <c r="B32" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>279</v>
+      </c>
+      <c r="C33" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>325</v>
+      </c>
+      <c r="F35">
+        <f>LEN(C36)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>570</v>
+      </c>
+      <c r="C36" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>571</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <f>LEN(C38)</f>
+        <v>104</v>
+      </c>
+      <c r="H37">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>438</v>
+      </c>
+      <c r="C38" t="str" cm="1">
+        <f t="array" ref="C38">AES_Encrypt(C33,C34,C35,C36,C37)</f>
+        <v>0E3FF3977F23489D4D320C8303F11E8A559ED3E16E5648E3049AC65A876E64A7A77C3C643737EBE03DD4BE8A901274F3C6F2D949</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="str" cm="1">
+        <f t="array" ref="C39">AES_Decrypt(C33,C38,C35,C36,C37)</f>
+        <v>486920416C69636520776861742061626F75742064696E6E657220746F6E69676874203F</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="C41" t="str" cm="1">
+        <f t="array" ref="C41">Util_HexStrToBase64(C38)</f>
+        <v>Dj/zl38jSJ1NMgyDA/EeilWe0+FuVkjjBJrGWoduZKenfDxkNzfr4D3UvoqQEnTz_x000D_
+xvLZSQ==</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6489,8 +6586,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:A60"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6549,7 +6646,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">RSA_Encrypt(C1,C3)</f>
-        <v>6DF6B98BE021A3A196401E2F2A69F27752EAC1B278E46D0ED82ED3F809100ABD6411B4ABB2D087F5FAD0521306E6BC01236EB655C66058951DC4A0AE5A3DE5C63A6B1D4EED645471AA2C8F26ECF9A1642CE88BF36115353ADBE402428A56691DA2FC5A17FCD1A8573507E4635419E846A566E135BA106ACCF5FBDF8A9B16C9CC1E03F3E45A4F0D61DBB195775C3BFA24D44FEF842B4C19D6593308E03A5F2F66DA580F78F427532672FE1DF337A5C7B8E4E505926E0FCD431CA1BBFB83AF0A69FFC37ED02D8AE4E81397B9C31F57FA36AEA5BE15591836B9761CFD464B0B288264A898D6273F0A33F94BE85F4720C92E9B48B09CEC2DF6F78722FC2BE08B6546</v>
+        <v>4A3010F111BFDDC8A4BE776DCE44C215B53E56DA935DDB6FE05D0470A6C8CD1FA6DAB0304671489E2ADF7FBF476F06B8B801C20D4307E95F4FE2F3C4E00B81737C6DBC76A152C610B706785F6DFDDCDBEC47671A83B4294D5FB7C2ACAD11E94FBF676FA9329658FCEA6C83A55756A74110FAE397D5BC0713431442D454B94D9608A1841D0A500D63B8C6F714ED86D9431432D01E534BC5E5DC176D51834CB24D8500485A3C539919A20A02C0EC1AB5E2A3292010F05F12B693516486938D4A84FC9A1B89B6B6D47C8756219F92C8E41392E7B9A021A629BF407F28AE6FACAB6957C02A6ED7BAE7618FA16BB2C70427741CC7881DEE26BF03665631FB33C6F67A</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6567,7 +6664,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6654,7 +6751,7 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">RSA_Encrypt(C10,C3,C11,C12,C13)</f>
-        <v>65ABE183B59FE818971A4453C62372E934A49CEB4CE2F267260DD3DBBEAA0F291E090E0E6F0871D19B78BE1275B95FC330590F4C8F6A39D12953F55A9C5806FD32D9D2BD85D9343B600DF5AB70F70544D72CDB2687AB73C2575316CA9E671423F8413086D65CB46887AD9DAF932B6B627E3B20B9EBEBE53941181964F916B4BE0917060C5AEB116465AF03FC8942C62DECE9CB8BE0DC039C0FEDA792CB603EC7D6F29A7608BAE2F3ABAC580A43F7BDFEEFABD1B86121232E18C75F244540A02387574A23475B0C89E1A0F495960C1B35AF9CD703DA06178A6C923F471666548BF13574EE76E96ABE2C3D2A1E3147B69E97C5A13A941A8FB968A37D4BA4C78140</v>
+        <v>436657D2D453D9C8ABFC48603789B0B399CAA9F3A1F2AFB5AFBA5435C1AEB3BD1FA7233FD62AD8E162065169433E35C5DF8D0104C9C2945B2F24D2B2B90206E4EE75B4B97B4ED0C696AD3DB5D34545A4FE026587EA5F440FE7895B6D5EAFACCADB8D28659F54BC1600CC8EBA436FA126A9A467983C4C971A19D0B8AD70E8DF6D709DDA097E5B9545E4650FCBF041D327E143549A6F81B6496B50B863C421B3AFEEEEB31FA688F956FEE42E3380DC8B0A8664426320364629EF308F8FE349898E1AB4932E3464C1F7D65277C98DCEEE59259AFFB59373250B1F8D76502F0B0F85CDF9F9A6153247EDA1A06FC02E6AE58F021420E8A509C36406ECB219C6CA1AD5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -6673,7 +6770,7 @@
     <row r="16" spans="1:3">
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">RSA_Encrypt(C1,C3,C11,C12,C13)</f>
-        <v>89A4FBA7E9071109A57903B42B599811607D93ADC52E14E44E0FA0E081C4D71E7061514319BFA9F9D21FD39ECC07CFFC3DC7621D776DBA8F5AA888CA94A8F8E3CA5FF5793390777FFFDA7B5ED21275CFA45819A9F409B4C31CF80D254C146A9107D5B83A2CB045E2D6398DD7DD22510D73A44D42921584384C0BFAC9BC68A18B5FDEDB7F43D35863A6E88972E18E975339E3D9DCFBEB12C1B4F5E2831D85EBBA8F97F75DAC376038C82A5593DD2D81A62D3288970A5871B79E79D25177CDA0548BE3732B94F48BB48D5EDE1A95900D9550A75ED2132E0813587934217C3155AA6EAE4852490EA55993D95B18D5CC72D8EC0C3C8D9542CF9123221CCB87C1F6F5</v>
+        <v>3D0FEB0195098E7AAA785E876A829CB252B41C7420A01CDD854CE99243ED29B57976820B47D14FD772545B2787B112AD858F5A1367F278FEF494837B8C0C106D7E03C9B8F4E86AF0DCBD4D7E5D9796F0EF3C7B93BFDB7105FDB4C55402341BAFB035A48B78BB94C34F1FFBADE35113B72AF6A45804B34142E2F1C56B8AEE6A32CE04EBFEA3E314BB179B46718D9BD69F3DA0B82E7DBFEBC8682237FF1318F2B15018468E7B0498F98456900558D5A8259A462FF077D45E131E4FF52419E509C7D526FE7E3D3D25A53E27BE5B1CE25170E9838B9826A08D25E3908ADB0DDD0F264B73E3002A90FA0DCC9781FBE8A17C7CB3B006F9AAAD177EDB5E02507678272A</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6684,7 +6781,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6701,7 +6798,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" ref="B20">Util_showFormula(C20)</f>
@@ -6713,7 +6810,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">Util_showFormula(C21)</f>
@@ -6730,7 +6827,7 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">RSA_Encrypt(C1,C3,C19,C20,C21)</f>
-        <v>7B0956F5CF6BEEE1BD9389ED49086F4448C27D3AC17161782957D1856AA1B133C91940CA5BCEC635DDAF978285C87AAD6D8509B452A083415022C17747B7557928CF8A5C6DC9FA23F14F8BC40C44909F67943FD9111BB07CCF8A0376672F02C9C4381DAA62F89393CEEA4BA619E92B5F3CDA7E641219EF9F346BC6BDB50DD1BA9CEB8BB102A4670F42133AAFE4FCF5F53BF286860A4B9AA634DAF3A9616BD370D4538D67EA764F14FFE2C5C0FF7B985515E861F05C571A54348E5DD8F8212B28C3F7CB86D62BD6A32F31B57C468A8A01A3ABCC9624034375139943C5AD7244A670E7458291C0FC6B440ADBCA13074FA1EB740EB22962F2E564A6DEF5377C42BD</v>
+        <v>6FE6368E71211F5541440F4B40EA00B034130095A450DAD4A75A348DFB9185A677B77359022AECE9677B1346148064A3B9627B94FAA4E511CFEBB8FA9E463E39474B15D3719D6FB240AE569B6B70D9684C0C109A540D4A5FAA00AD45778715D368838ECE12E81791BD467E0A374C9B6D45FEB4C1A47D95F0BFDD26077AC469687F56CDE457AF23A4223EFBA94A0B43C48D302CF42A8F7767A2422EC26E16E8DB333329C4FE39710A00877741FD143216301BC0B98BBE8D332EC0FD1C4CEA06C5EEC670874CF0239D2360ECB5C2F0E27B4EF69B9D403209113F4F297C95291FD8F252E897923E8678B918905B4B014EB45C3248456AE991F68D30C05E3A6B8A6F</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -6748,7 +6845,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26">Util_showFormula(C26)</f>
@@ -6756,22 +6853,22 @@
       </c>
       <c r="C26" t="str" cm="1">
         <f t="array" ref="C26">Util_HexStrToBase64(C22)</f>
-        <v>ewlW9c9r7uG9k4ntSQhvREjCfTrBcWF4KVfRhWqhsTPJGUDKW87GNd2vl4KFyHqt_x000D_
-bYUJtFKgg0FQIsF3R7dVeSjPilxtyfoj8U+LxAxEkJ9nlD/ZERuwfM+KA3ZnLwLJ_x000D_
-xDgdqmL4k5PO6kumGekrXzzafmQSGe+fNGvGvbUN0bqc64uxAqRnD0ITOq/k/PX1_x000D_
-O/KGhgpLmqY02vOpYWvTcNRTjWfqdk8U/+LFwP97mFUV6GHwXFcaVDSOXdj4ISso_x000D_
-w/fLhtYr1qMvMbV8RoqKAaOrzJYkA0N1E5lDxa1yRKZw50WCkcD8a0QK28oTB0+h_x000D_
-63QOsili8uVkpt71N3xCvQ==</v>
+        <v>b+Y2jnEhH1VBRA9LQOoAsDQTAJWkUNrUp1o0jfuRhaZ3t3NZAirs6Wd7E0YUgGSj_x000D_
+uWJ7lPqk5RHP67j6nkY+OUdLFdNxnW+yQK5Wm2tw2WhMDBCaVA1KX6oArUV3hxXT_x000D_
+aIOOzhLoF5G9Rn4KN0ybbUX+tMGkfZXwv90mB3rEaWh/Vs3kV68jpCI++6lKC0PE_x000D_
+jTAs9CqPd2eiQi7Cbhbo2zMzKcT+OXEKAId3Qf0UMhYwG8C5i76NMy7A/RxM6gbF_x000D_
+7sZwh0zwI50jYOy1wvDie072m51AMgkRP08pfJUpH9jyUuiXkj6GeLkYkFtLAU60_x000D_
+XDJIRWrpkfaNMMBeOmuKbw==</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K29" s="3"/>
     </row>
@@ -6780,7 +6877,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -6811,7 +6908,7 @@
         <v>0LGGUE50v76TPaYzwH+CIphVRwcDFE3YOnhelUlBycz8uxQbf2tTW/wHJyjbjtMnaXkAlB7Dkv5gU2haEeHXJyMqU+SNxj4B/oa+Mbl8l59sjPzWaxPMUX9j3gOzCqxZhbCCfZ6uObo9rFaZXcdYoFIZnNZbrgZUGXG39E2ju5yXFK6pPGU9t5lFY/oXAKgxE7FP3qynusXnPXYlJuh3pQtg0pTrJbwUcWB6cBnyfEXZajehI5hbLOTODmxIvJ/HhTS34L3QlzbOXDCwro9Mkrmx6qOK/wDuFZfTnmSZTOQZdSnYlKklLqutMQdm53AVJkAJUsC8vGjS/JL6h1tOQg==</v>
       </c>
       <c r="C33" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -6819,7 +6916,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B34" t="str" cm="1">
         <f t="array" ref="B34">Util_showFormula(C34)</f>
@@ -6862,7 +6959,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B37" t="str" cm="1">
         <f t="array" ref="B37">Util_showFormula(C37)</f>
@@ -6877,7 +6974,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B38" t="str" cm="1">
         <f t="array" ref="B38">Util_showFormula(C38)</f>
@@ -6892,7 +6989,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B39" t="str" cm="1">
         <f t="array" ref="B39">Util_showFormula(C39)</f>
@@ -6911,7 +7008,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -7320,7 +7417,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -7559,7 +7656,7 @@
         <v>prime256v1</v>
       </c>
       <c r="C8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -7625,7 +7722,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -7694,7 +7791,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C21" t="s">
         <v>95</v>
@@ -7712,10 +7809,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>387</v>
+      </c>
+      <c r="C23" t="s">
         <v>388</v>
-      </c>
-      <c r="C23" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -7730,7 +7827,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" ref="B25">Util_showFormula(C25)</f>
@@ -7743,7 +7840,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26">Util_showFormula(C26)</f>
@@ -7756,14 +7853,14 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27">Util_showFormula(C27)</f>
         <v>HASH</v>
       </c>
       <c r="C27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -7804,7 +7901,7 @@
         <v>4865726520697320736F6D65206F7468657220696E666F0A</v>
       </c>
       <c r="I30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -7847,7 +7944,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B35" t="str" cm="1">
         <f t="array" ref="B35">Util_showFormula(C35)</f>
@@ -7860,7 +7957,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B36" t="str" cm="1">
         <f t="array" ref="B36">Util_showFormula(C36)</f>
@@ -7873,14 +7970,14 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B37" t="str" cm="1">
         <f t="array" ref="B37">Util_showFormula(C37)</f>
         <v>RAW</v>
       </c>
       <c r="C37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -7955,24 +8052,24 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B48" t="str" cm="1">
         <f t="array" ref="B48">Util_showFormula(C48)</f>
         <v>MEYCIQDwOh0NpUfBWMdSuj7a6fiQMR1o3yCM227HGgKmeUwYcQIhAMzxXZatKbQ5HqsX+YHgyxQGW9+fAgOUtH7+sVZ2Z9Gz</v>
       </c>
       <c r="C48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="C49" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -8033,31 +8130,31 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B55" t="str" cm="1">
         <f t="array" ref="B55">Util_showFormula(C55)</f>
         <v>DER</v>
       </c>
       <c r="C55" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B56" t="str" cm="1">
         <f t="array" ref="B56">Util_showFormula(C56)</f>
         <v>OK</v>
       </c>
       <c r="C56" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B57" t="str" cm="1">
         <f t="array" ref="B57">Util_showFormula(C57)</f>
@@ -8070,7 +8167,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -8126,19 +8223,19 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B66" t="str" cm="1">
         <f t="array" ref="B66">Util_showFormula(C66)</f>
         <v>DER</v>
       </c>
       <c r="C66" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B67" t="str" cm="1">
         <f t="array" ref="B67">Util_showFormula(C67)</f>
@@ -8146,12 +8243,12 @@
       </c>
       <c r="C67" t="str" cm="1">
         <f t="array" ref="C67">EC_SignHash(C64,C65,C66)</f>
-        <v>3044022011799736B67CEEC699DBF4F9995AEC9AF3219B8F13357548885C77E44277213702202A9916E4B4E9C10ECE39625D923CF1B79ABFDA6A3FB26FA32CEE38863C97CFB3</v>
+        <v>3046022100A6C41900021D0D90F72D731B09273A027400802480AD502CB870CB10EA4915D3022100EB1D2D79FD5A963773404BEC8A5615C7537A0D3D2174BF5348B8C336A721F673</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B68" t="str" cm="1">
         <f t="array" ref="B68">Util_showFormula(C68)</f>
@@ -8159,18 +8256,18 @@
       </c>
       <c r="C68" t="str" cm="1">
         <f t="array" ref="C68">Util_HexStrToBase64(C67)</f>
-        <v>MEQCIBF5lza2fO7Gmdv0+Zla7JrzIZuPEzV1SIhcd+RCdyE3AiAqmRbktOnBDs45_x000D_
-Yl2SPPG3mr/aaj+yb6Ms7jiGPJfPsw==</v>
+        <v>MEYCIQCmxBkAAh0NkPctcxsJJzoCdACAJICtUCy4cMsQ6kkV0wIhAOsdLXn9WpY3_x000D_
+c0BL7IpWFcdTeg09IXS/U0i4wzanIfZz</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="C73" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KCV calc for AES and DES
</commit_message>
<xml_diff>
--- a/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
+++ b/ExcelExampleAndMakroSource/ExcelCryptoNoMacro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88215cb98efcb80/Documents/Excel experiments/ExcelExampleAndMakroSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{D495C800-C295-49CE-B013-35DFA772AE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50037885-D4B8-4AA1-A789-410D2C790364}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D11315F8-8B15-4537-9D35-2118881B8711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{195B1F65-E573-4273-AC4C-689BB3C4FCB7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="584">
   <si>
     <t>Plain</t>
   </si>
@@ -1997,6 +1997,36 @@
   </si>
   <si>
     <t>Public Function AES_Encrypt(ByVal key As String, ByVal plain As String, Optional ByVal mode As String = "CBC", Optional ByVal iv As String = "", Optional ByVal GCMtagLen As Long = 12) As String</t>
+  </si>
+  <si>
+    <t>DES_KCV</t>
+  </si>
+  <si>
+    <t>Hex00x8</t>
+  </si>
+  <si>
+    <t>AES_KCV</t>
+  </si>
+  <si>
+    <t>Hex00x16</t>
+  </si>
+  <si>
+    <t>------------------------------------------------------------------------------------------------------_x000D_
+' AES_KCV (key) calculate a KCV i.e. encrypt 8*x00 with IV 0x00 and return first 4 bytes_x000D_
+' key           : The DES key in hex string can be single DES, Double DES or Tripple DES_x000D_
+'------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Public Function AES_KCV(ByVal key As String, Optional ByVal kcvLen As Long = 8) As String</t>
+  </si>
+  <si>
+    <t>------------------------------------------------------------------------------------------------------_x000D_
+' DES_KCV (key) calculate a KCV i.e. encrypt 8*x00 with IV 0x00 and return first 4 bytes_x000D_
+' key           : The DES key in hex string can be single DES, Double DES or Tripple DES_x000D_
+'------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Public Function DES_KCV(ByVal key As String, Optional ByVal kcvLen As Long = 8) As String</t>
   </si>
 </sst>
 </file>
@@ -3908,275 +3938,291 @@
         <v>367</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="108.6">
+    <row r="17" spans="1:3" ht="60.6">
       <c r="A17" t="s">
-        <v>232</v>
+        <v>578</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>518</v>
+        <v>580</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>368</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="108.6">
       <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="108.6">
+      <c r="A19" t="s">
         <v>233</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B19" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="96.6">
-      <c r="A19" t="s">
-        <v>476</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>520</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="96.6">
+    <row r="20" spans="1:3" ht="60.6">
       <c r="A20" t="s">
-        <v>477</v>
+        <v>576</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>522</v>
+        <v>582</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>523</v>
+        <v>583</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="96.6">
       <c r="A21" t="s">
+        <v>476</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="96.6">
+      <c r="A22" t="s">
+        <v>477</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="96.6">
+      <c r="A23" t="s">
         <v>478</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>524</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="84.6">
-      <c r="A22" t="s">
+    <row r="24" spans="1:3" ht="84.6">
+      <c r="A24" t="s">
         <v>479</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B24" s="15" t="s">
         <v>525</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="72.599999999999994">
-      <c r="A23" t="s">
+    <row r="25" spans="1:3" ht="72.599999999999994">
+      <c r="A25" t="s">
         <v>480</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B25" s="15" t="s">
         <v>527</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C25" s="18" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="72.599999999999994">
-      <c r="A24" t="s">
+    <row r="26" spans="1:3" ht="72.599999999999994">
+      <c r="A26" t="s">
         <v>481</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B26" s="15" t="s">
         <v>528</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="84.6">
-      <c r="A25" t="s">
-        <v>482</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="84.6">
-      <c r="A26" t="s">
-        <v>483</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>530</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="84.6">
       <c r="A27" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="84.6">
       <c r="A28" t="s">
+        <v>483</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="84.6">
+      <c r="A29" t="s">
+        <v>484</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="84.6">
+      <c r="A30" t="s">
         <v>485</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B30" s="15" t="s">
         <v>532</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C30" s="18" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="72.599999999999994">
-      <c r="A29" t="s">
-        <v>493</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="72.599999999999994">
-      <c r="A30" t="s">
-        <v>487</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>534</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="72.599999999999994">
       <c r="A31" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="72.599999999999994">
       <c r="A32" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>363</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="72.599999999999994">
       <c r="A33" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>421</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="72.599999999999994">
       <c r="A34" t="s">
+        <v>489</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="72.599999999999994">
+      <c r="A35" t="s">
+        <v>491</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>537</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="72.599999999999994">
+      <c r="A36" t="s">
         <v>492</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>538</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C36" s="17" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="84.6">
-      <c r="A35" t="s">
+    <row r="37" spans="1:3" ht="84.6">
+      <c r="A37" t="s">
         <v>370</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B37" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C37" s="18" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="84.6">
-      <c r="A36" t="s">
+    <row r="38" spans="1:3" ht="84.6">
+      <c r="A38" t="s">
         <v>495</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B38" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C38" s="18" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="108.6">
-      <c r="A37" t="s">
+    <row r="39" spans="1:3" ht="108.6">
+      <c r="A39" t="s">
         <v>496</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B39" s="15" t="s">
         <v>541</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C39" s="18" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="108.6">
-      <c r="A38" t="s">
+    <row r="40" spans="1:3" ht="108.6">
+      <c r="A40" t="s">
         <v>490</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B40" s="15" t="s">
         <v>542</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="96.6">
-      <c r="A39" t="s">
+    <row r="41" spans="1:3" ht="96.6">
+      <c r="A41" t="s">
         <v>486</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>544</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C41" s="18" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="72.599999999999994">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3" ht="72.599999999999994">
+      <c r="A42" t="s">
         <v>494</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B42" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="B42" s="15"/>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" s="15"/>
@@ -4260,7 +4306,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">Util_GenRandom(32)</f>
-        <v>E62B9DE0FBFD8C9D80E010B4742C370262A75131C8FB2A40AE1A18EB3C41AE58</v>
+        <v>C735811C116EC0204E85E6766311857D673CB98310635F40B237C5411D288DE0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4278,7 +4324,7 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">Util_GenRandom((16))</f>
-        <v>169F6AA1D13E75824C3B1FBB06F3F8D7</v>
+        <v>4EEEE1589CD4C0BE00DCE2E16E35C8BD</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4291,7 +4337,7 @@
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">Util_HexStrToBase64(C9)</f>
-        <v>Fp9qodE+dYJMOx+7BvP41w==</v>
+        <v>Tu7hWJzUwL4A3OLhbjXIvQ==</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4338,7 +4384,7 @@
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">AES_Encrypt(C7,C13,C14,C9)</f>
-        <v>BBA8318AC4F3ECBF823680F681F14CF8BE7A4661F02C5FA7E2F2A47052B05B90822EF3EA0F9C0A24464AAE9031C4B982</v>
+        <v>FC4F87B334DE2C51E125BA7BDCF5AA7CA9C7E7CF6F0DBB13CDBD6F9DB71BFDD930D80C07B99AE9C1E895F28AC7FFFEC6</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4351,7 +4397,7 @@
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">Util_HexStrToBase64(C16)</f>
-        <v>u6gxisTz7L+CNoD2gfFM+L56RmHwLF+n4vKkcFKwW5CCLvPqD5wKJEZKrpAxxLmC</v>
+        <v>/E+HszTeLFHhJbp73PWqfKnH589vDbsTzb1vnbcb/dkw2AwHuZrpweiV8orH//7G</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4465,7 +4511,7 @@
       </c>
       <c r="C31" t="str" cm="1">
         <f t="array" ref="C31">RSA_Encrypt(C29,C7,C30)</f>
-        <v>6C3822787D0389B2E080927048283B81C31121A4F18BBE50C5532D9F6033B3F56FCCFDC678DC977C5896AC7C200C6A0116B347E8526B0378B824DEE43DBE2D659CE85FB5B3D9EBB4D69CE8040B7F81EBED9B7F73E1A0BBC3A556DA45CF83C47D1B49BFFF24B6880782D28384BB6AD9C22D61E65B0F6DD73F24F1965920BFA89D5A24A38EA1A1C479B3E4EDE326AE420E6C191E1E1D18906958A032C7140B05F2DB3468063704143A5FB842E6A31FFC2DDDC5A3D18CE89A3681256A0F75F9804A0E8B484DA061DF4536748A50E87258270A9C41C2EAE11F196C7FD4308B01DBDD177AD822FDB798C83F5A8C697399B0CFF9987AF0E5E351FBDB5B191118533C26</v>
+        <v>95814574266B1D1B4D0B9F2E6DAE28225F728F9C3A5ADF6B3CA5CBEC72D0B94217F6D5C4F152C91479ACC6ED423096FAB4991C9CD6104FE7AE7D0E125EF74B9B29BEDECDCD8348F088EB486CA373CDA5BDED9EA694E2E719A4A8FCA5980E8C52D7FAE0C53D936DEDC50A4977DE07F1D0A72DB6E821496A1CD4C974606503FEB50B541C56C54FC9CE55973DEE815EE16AEEF068B6F17C0C98844949901F08B3DD9BD9BD0C70749F214310454AEE30A42EAE93E20C31DB066F4E6E39B72DE642C324231CA07C6BBC06C62D9FC2C51E8DE7B56E7C291123E1205F2F396DFCF5AB702C19BBBB00056E41BDD05B392C62CDBA3E21C2FEA1C6DB64353EF59A3C9B49D6</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4478,12 +4524,12 @@
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">Util_HexStrToBase64(C31)</f>
-        <v>bDgieH0DibLggJJwSCg7gcMRIaTxi75QxVMtn2Azs/VvzP3GeNyXfFiWrHwgDGoB_x000D_
-FrNH6FJrA3i4JN7kPb4tZZzoX7Wz2eu01pzoBAt/gevtm39z4aC7w6VW2kXPg8R9_x000D_
-G0m//yS2iAeC0oOEu2rZwi1h5lsPbdc/JPGWWSC/qJ1aJKOOoaHEebPk7eMmrkIO_x000D_
-bBkeHh0YkGlYoDLHFAsF8ts0aAY3BBQ6X7hC5qMf/C3dxaPRjOiaNoElag91+YBK_x000D_
-DotITaBh30U2dIpQ6HJYJwqcQcLq4R8ZbH/UMIsB290Xetgi/beYyD9ajGlzmbDP_x000D_
-+Zh68OXjUfvbWxkRGFM8Jg==</v>
+        <v>lYFFdCZrHRtNC58uba4oIl9yj5w6Wt9rPKXL7HLQuUIX9tXE8VLJFHmsxu1CMJb6_x000D_
+tJkcnNYQT+eufQ4SXvdLmym+3s3Ng0jwiOtIbKNzzaW97Z6mlOLnGaSo/KWYDoxS_x000D_
+1/rgxT2Tbe3FCkl33gfx0KcttughSWoc1Ml0YGUD/rULVBxWxU/JzlWXPe6BXuFq_x000D_
+7vBotvF8DJiESUmQHwiz3ZvZvQxwdJ8hQxBFSu4wpC6uk+IMMdsGb05uObct5kLD_x000D_
+JCMcoHxrvAbGLZ/CxR6N57VufCkRI+EgXy85bfz1q3AsGbu7AAVuQb3QWzksYs26_x000D_
+PiHC/qHG22Q1PvWaPJtJ1g==</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4502,7 +4548,7 @@
       </c>
       <c r="C35" t="str">
         <f>C10</f>
-        <v>Fp9qodE+dYJMOx+7BvP41w==</v>
+        <v>Tu7hWJzUwL4A3OLhbjXIvQ==</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4516,7 +4562,7 @@
       </c>
       <c r="C36" t="str">
         <f>C17</f>
-        <v>u6gxisTz7L+CNoD2gfFM+L56RmHwLF+n4vKkcFKwW5CCLvPqD5wKJEZKrpAxxLmC</v>
+        <v>/E+HszTeLFHhJbp73PWqfKnH589vDbsTzb1vnbcb/dkw2AwHuZrpweiV8orH//7G</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4530,12 +4576,12 @@
       </c>
       <c r="C37" t="str">
         <f>C32</f>
-        <v>bDgieH0DibLggJJwSCg7gcMRIaTxi75QxVMtn2Azs/VvzP3GeNyXfFiWrHwgDGoB_x000D_
-FrNH6FJrA3i4JN7kPb4tZZzoX7Wz2eu01pzoBAt/gevtm39z4aC7w6VW2kXPg8R9_x000D_
-G0m//yS2iAeC0oOEu2rZwi1h5lsPbdc/JPGWWSC/qJ1aJKOOoaHEebPk7eMmrkIO_x000D_
-bBkeHh0YkGlYoDLHFAsF8ts0aAY3BBQ6X7hC5qMf/C3dxaPRjOiaNoElag91+YBK_x000D_
-DotITaBh30U2dIpQ6HJYJwqcQcLq4R8ZbH/UMIsB290Xetgi/beYyD9ajGlzmbDP_x000D_
-+Zh68OXjUfvbWxkRGFM8Jg==</v>
+        <v>lYFFdCZrHRtNC58uba4oIl9yj5w6Wt9rPKXL7HLQuUIX9tXE8VLJFHmsxu1CMJb6_x000D_
+tJkcnNYQT+eufQ4SXvdLmym+3s3Ng0jwiOtIbKNzzaW97Z6mlOLnGaSo/KWYDoxS_x000D_
+1/rgxT2Tbe3FCkl33gfx0KcttughSWoc1Ml0YGUD/rULVBxWxU/JzlWXPe6BXuFq_x000D_
+7vBotvF8DJiESUmQHwiz3ZvZvQxwdJ8hQxBFSu4wpC6uk+IMMdsGb05uObct5kLD_x000D_
+JCMcoHxrvAbGLZ/CxR6N57VufCkRI+EgXy85bfz1q3AsGbu7AAVuQb3QWzksYs26_x000D_
+PiHC/qHG22Q1PvWaPJtJ1g==</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -4861,7 +4907,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">Util_GenRandom(32)</f>
-        <v>A6893B147B859F4865A4F9688361DFD7750E1D2FC31BF9A61995D6DFF9342639</v>
+        <v>3EF768372FBA423211AFEA1958BED11E6BC9EC38EF51DE27E5E0D22DEF9D9A86</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4879,7 +4925,7 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">Util_GenRandom((12))</f>
-        <v>319012BC1DA1734ACB44E881</v>
+        <v>E6CBFE9283C32EAED343EB8C</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -4892,7 +4938,7 @@
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">Util_HexStrToBase64(C9)</f>
-        <v>MZASvB2hc0rLROiB</v>
+        <v>5sv+koPDLq7TQ+uM</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -4939,7 +4985,7 @@
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">AES_Encrypt(C7,C13,C14,C9)</f>
-        <v>9E6480D973EBFCA33F35D717B1B99DAEA3A40C49DC9823A4050C5FD1843890319898ED5810414162EBFC6C1EB29E1386</v>
+        <v>098E217F52406E594565DA77B642EFF66BFD21BB65AB870B00F5BDDC6EB9F7EEA93DA788D5AE51A897BF0907A2B91450</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4957,7 +5003,7 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">Util_HexStrToBase64(C16)</f>
-        <v>nmSA2XPr/KM/NdcXsbmdrqOkDEncmCOkBQxf0YQ4kDGYmO1YEEFBYuv8bB6ynhOG</v>
+        <v>CY4hf1JAbllFZdp3tkLv9mv9Ibtlq4cLAPW93G659+6pPaeI1a5RqJe/CQeiuRRQ</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4972,7 +5018,7 @@
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">GCM_getEncrypted(C16)</f>
-        <v>9E6480D973EBFCA33F35D717B1B99DAEA3A40C49DC9823A4050C5FD1843890319898ED58</v>
+        <v>098E217F52406E594565DA77B642EFF66BFD21BB65AB870B00F5BDDC6EB9F7EEA93DA788</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4982,7 +5028,7 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">GCM_getTag(C16)</f>
-        <v>10414162EBFC6C1EB29E1386</v>
+        <v>D5AE51A897BF0907A2B91450</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5122,7 +5168,7 @@
       </c>
       <c r="C39" t="str" cm="1">
         <f t="array" ref="C39">RSA_Encrypt(C34,C7,C35,C36,C37)</f>
-        <v>64C0FB287838A1B0168A7AEA97E3CBB3B66AFDD5338DF02FBB497095159F4CBBBCC54575DB60027B569C4FDA5A786D23E7C37CC8124A8C40DD5DCD6270DAD5EFC7FFB8B68A9148A2E60E6F0A762ECC6EC19A4481D6FD32040FF7CB685CA07D363F240090BE21416AFABECB1B2CFBC2DE3BAF3720CFDB294DD5FEBA99F1CB101DDD47E959204B754CF46E993C3374BB91A9F15A2616407B9BB804E2ADE1B8ADC98F6F6F35DD3E4B92115CA3E9C601B373E95CD55E0D546BEDEC033DA5A6245A870EF497C303C6A1391F722F9D25D9EB63C884809FA217616B280F9ECC96D2C4BA424331E030CF12ACF3736FB5A9CD4415EFF89726D9E7DDFB7B3BD84DD0BB1A57</v>
+        <v>8E83E877D9AA8FD215823A02625B7B4192E5B91665F21919B15E5C9D10D0CD20A2F42D25BAF80A74012E4AF8C76C6DA4DCFC12D2E95D372E7C1282311AF7B44197F5B576A783CDD4649A4D6C7EFD920886F081ABC473E55AA203D40638E2BD6B54717621A1C786315095D4D4BABC361D27E45C85058C2343DB12276D11F045412133AB436024FF32239AA780D653B131358A0987DAEB88D6AB00D610F36C96802F2AB75D80F11741604D959ECEEB600AA0E7DF42826980D169A36B26FE5DDDA660852F63D65E85F5A8973E96B58C38D63D42B2C2BDAD8278F1DFEB909146BCA57537F9647A44A734F83509B4FB5B2D99935EA78982EBA2AE64C0C7A87475C2F5</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5135,12 +5181,12 @@
       </c>
       <c r="C40" t="str" cm="1">
         <f t="array" ref="C40">Util_HexStrToBase64(C39)</f>
-        <v>ZMD7KHg4obAWinrql+PLs7Zq/dUzjfAvu0lwlRWfTLu8xUV122ACe1acT9paeG0j_x000D_
-58N8yBJKjEDdXc1icNrV78f/uLaKkUii5g5vCnYuzG7BmkSB1v0yBA/3y2hcoH02_x000D_
-PyQAkL4hQWr6vssbLPvC3juvNyDP2ylN1f66mfHLEB3dR+lZIEt1TPRumTwzdLuR_x000D_
-qfFaJhZAe5u4BOKt4bityY9vbzXdPkuSEVyj6cYBs3PpXNVeDVRr7ewDPaWmJFqH_x000D_
-DvSXwwPGoTkfci+dJdnrY8iEgJ+iF2FrKA+ezJbSxLpCQzHgMM8SrPNzb7WpzUQV_x000D_
-7/iXJtnn3ft7O9hN0LsaVw==</v>
+        <v>joPod9mqj9IVgjoCYlt7QZLluRZl8hkZsV5cnRDQzSCi9C0luvgKdAEuSvjHbG2k_x000D_
+3PwS0uldNy58EoIxGve0QZf1tXang83UZJpNbH79kgiG8IGrxHPlWqID1AY44r1r_x000D_
+VHF2IaHHhjFQldTUurw2HSfkXIUFjCND2xInbRHwRUEhM6tDYCT/MiOap4DWU7Ex_x000D_
+NYoJh9rriNarANYQ82yWgC8qt12A8RdBYE2Vns7rYAqg599CgmmA0Wmjayb+Xd2m_x000D_
+YIUvY9ZehfWolz6WtYw41j1CssK9rYJ48d/rkJFGvKV1N/lkekSnNPg1CbT7Wy2Z_x000D_
+k16niYLroq5kwMeodHXC9Q==</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -5158,7 +5204,7 @@
       </c>
       <c r="C43" t="str">
         <f>C10</f>
-        <v>MZASvB2hc0rLROiB</v>
+        <v>5sv+koPDLq7TQ+uM</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -5172,7 +5218,7 @@
       </c>
       <c r="C44" t="str">
         <f>C18</f>
-        <v>nmSA2XPr/KM/NdcXsbmdrqOkDEncmCOkBQxf0YQ4kDGYmO1YEEFBYuv8bB6ynhOG</v>
+        <v>CY4hf1JAbllFZdp3tkLv9mv9Ibtlq4cLAPW93G659+6pPaeI1a5RqJe/CQeiuRRQ</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -5219,12 +5265,12 @@
       </c>
       <c r="C47" t="str">
         <f>C40</f>
-        <v>ZMD7KHg4obAWinrql+PLs7Zq/dUzjfAvu0lwlRWfTLu8xUV122ACe1acT9paeG0j_x000D_
-58N8yBJKjEDdXc1icNrV78f/uLaKkUii5g5vCnYuzG7BmkSB1v0yBA/3y2hcoH02_x000D_
-PyQAkL4hQWr6vssbLPvC3juvNyDP2ylN1f66mfHLEB3dR+lZIEt1TPRumTwzdLuR_x000D_
-qfFaJhZAe5u4BOKt4bityY9vbzXdPkuSEVyj6cYBs3PpXNVeDVRr7ewDPaWmJFqH_x000D_
-DvSXwwPGoTkfci+dJdnrY8iEgJ+iF2FrKA+ezJbSxLpCQzHgMM8SrPNzb7WpzUQV_x000D_
-7/iXJtnn3ft7O9hN0LsaVw==</v>
+        <v>joPod9mqj9IVgjoCYlt7QZLluRZl8hkZsV5cnRDQzSCi9C0luvgKdAEuSvjHbG2k_x000D_
+3PwS0uldNy58EoIxGve0QZf1tXang83UZJpNbH79kgiG8IGrxHPlWqID1AY44r1r_x000D_
+VHF2IaHHhjFQldTUurw2HSfkXIUFjCND2xInbRHwRUEhM6tDYCT/MiOap4DWU7Ex_x000D_
+NYoJh9rriNarANYQ82yWgC8qt12A8RdBYE2Vns7rYAqg599CgmmA0Wmjayb+Xd2m_x000D_
+YIUvY9ZehfWolz6WtYw41j1CssK9rYJ48d/rkJFGvKV1N/lkekSnNPg1CbT7Wy2Z_x000D_
+k16niYLroq5kwMeodHXC9Q==</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5659,7 +5705,7 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">Util_GenRandom(16)</f>
-        <v>F5F4B248D223D729A4963CEA69484697</v>
+        <v>90F35BC2F25721615684E984E99D7F1C</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5672,7 +5718,7 @@
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">AES_Encrypt(C11,C16,C17,C18)</f>
-        <v>C7749A9B22A78CD40C44A1745039752BB1FBB26141609F9E1A1A3A4BDE067D69D239F80E42B4D79F38DFCCEEF1065011F57D15BAD745DB1F3BBAA1BED0D77E47</v>
+        <v>19F987386FB4662FD7A0919BC5270C02AE0F4A44321D65713FA31595CB8042D538D196F43B7168974F1493F466050AE9D41AAE3763538C87FA8DA5161AD1F651</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -5753,7 +5799,7 @@
       </c>
       <c r="C28" t="str" cm="1">
         <f t="array" ref="C28">EC_SignHash(C25,C26,C27)</f>
-        <v>30440220289ECCD3A98AD9C381C95225640D4F8ACB72B461ED98B40F6BAE3AC7796675A30220644EBA1ADAF12856300F6F3915122B2861DD0E80FC2254135A569DD55A556447</v>
+        <v>3045022100EC297C4C15DE92C4828D69193E5130E896F2EEFA9E82CEFBCB2B6BAE94BF2B2B02206BF043A547D7FA5608E57E82BBBEAD180F1713FDC5733A43E7FAA5622E07C349</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -5784,8 +5830,8 @@
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">Util_HexStrToBase64(C19)</f>
-        <v>x3SamyKnjNQMRKF0UDl1K7H7smFBYJ+eGho6S94GfWnSOfgOQrTXnzjfzO7xBlAR_x000D_
-9X0VutdF2x87uqG+0Nd+Rw==</v>
+        <v>GfmHOG+0Zi/XoJGbxScMAq4PSkQyHWVxP6MVlcuAQtU40Zb0O3Fol08Uk/RmBQrp_x000D_
+1BquN2NTjIf6jaUWGtH2UQ==</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -5798,7 +5844,7 @@
       </c>
       <c r="C36" t="str" cm="1">
         <f t="array" ref="C36">Util_HexStrToBase64(C18)</f>
-        <v>9fSySNIj1ymkljzqaUhGlw==</v>
+        <v>kPNbwvJXIWFWhOmE6Z1/HA==</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -5811,8 +5857,8 @@
       </c>
       <c r="C37" t="str" cm="1">
         <f t="array" ref="C37">Util_HexStrToBase64(C28)</f>
-        <v>MEQCICiezNOpitnDgclSJWQNT4rLcrRh7Zi0D2uuOsd5ZnWjAiBkTroa2vEoVjAP_x000D_
-bzkVEisoYd0OgPwiVBNaVp3VWlVkRw==</v>
+        <v>MEUCIQDsKXxMFd6SxIKNaRk+UTDolvLu+p6CzvvLK2uulL8rKwIga/BDpUfX+lYI_x000D_
+5X6Cu76tGA8XE/3FczpD5/qlYi4Hw0k=</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -6131,20 +6177,18 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
@@ -6152,10 +6196,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -6165,13 +6208,9 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="str">
+      <c r="C3" s="6" t="str">
         <f>E3</f>
         <v>2b7e151628aed2a6abf7158809cf4f3c</v>
-      </c>
-      <c r="C3" s="3">
-        <f>LEN(B3)</f>
-        <v>32</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
@@ -6185,13 +6224,9 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="str">
+      <c r="C4" s="6" t="str">
         <f>E4</f>
         <v>000102030405060708090A0B0C0D0E0F</v>
-      </c>
-      <c r="C4" s="3">
-        <f>LEN(B4)</f>
-        <v>32</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
@@ -6206,11 +6241,10 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="str">
+      <c r="C5" s="6" t="str">
         <f>E5</f>
         <v>6bc1bee22e409f96e93d7e117393172a</v>
       </c>
-      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -6224,13 +6258,13 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="str" cm="1">
-        <f t="array" ref="B6">AES_Encrypt(B3,B5,B2,B4)</f>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6">Util_showFormula(C6)</f>
+        <v>=AES_Encrypt(C3,C5,C2,C4)</v>
+      </c>
+      <c r="C6" s="7" t="str" cm="1">
+        <f t="array" ref="C6">AES_Encrypt(C3,C5,C2,C4)</f>
         <v>7649ABAC8119B246CEE98E9B12E9197D8964E0B149C10B7B682E6E39AAEB731C</v>
-      </c>
-      <c r="C6" s="3">
-        <f>LEN(B6)</f>
-        <v>64</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
@@ -6245,11 +6279,14 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="str" cm="1">
-        <f t="array" ref="B7">AES_Decrypt(B3,B6,B2,B4)</f>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7">Util_showFormula(C7)</f>
+        <v>=AES_Decrypt(C3,C6,C2,C4)</v>
+      </c>
+      <c r="C7" s="7" t="str" cm="1">
+        <f t="array" ref="C7">AES_Decrypt(C3,C6,C2,C4)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
-      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" t="str">
@@ -6261,18 +6298,15 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="6"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -6284,11 +6318,10 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="str">
+      <c r="C11" s="3" t="str">
         <f>E11</f>
         <v>6bc1bee22e409f96e93d7e117393172a</v>
       </c>
-      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="5" t="s">
         <v>13</v>
@@ -6301,11 +6334,10 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="str">
+      <c r="C12" s="3" t="str">
         <f>E12</f>
         <v>2b7e151628aed2a6abf7158809cf4f3c</v>
       </c>
-      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="5" t="s">
         <v>11</v>
@@ -6315,21 +6347,19 @@
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3" t="str">
+      <c r="C14" s="3" t="str">
         <f>E14</f>
         <v>000102030405060708090A0B0C0D0E0F</v>
       </c>
-      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="5" t="s">
         <v>12</v>
@@ -6340,11 +6370,14 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="str" cm="1">
-        <f t="array" ref="B15">AES_Encrypt(B12,B11,B13,B14)</f>
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15">Util_showFormula(C15)</f>
+        <v>=AES_Encrypt(C12,C11,C13,C14)</v>
+      </c>
+      <c r="C15" s="3" t="str" cm="1">
+        <f t="array" ref="C15">AES_Encrypt(C12,C11,C13,C14)</f>
         <v>7649ABAC8119B246CEE98E9B12E9197D8964E0B149C10B7B682E6E39AAEB731C</v>
       </c>
-      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="5" t="s">
         <v>14</v>
@@ -6355,17 +6388,19 @@
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3" t="str" cm="1">
-        <f t="array" ref="B16">AES_Decrypt(B12,B15,B13,B14)</f>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16">Util_showFormula(C16)</f>
+        <v>=AES_Decrypt(C12,C15,C13,C14)</v>
+      </c>
+      <c r="C16" s="3" t="str" cm="1">
+        <f t="array" ref="C16">AES_Decrypt(C12,C15,C13,C14)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
-      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -6375,7 +6410,7 @@
       <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="2"/>
@@ -6384,8 +6419,8 @@
       <c r="A19" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3" t="str">
-        <f>B11</f>
+      <c r="C19" s="3" t="str">
+        <f>C11</f>
         <v>6bc1bee22e409f96e93d7e117393172a</v>
       </c>
       <c r="G19" s="2"/>
@@ -6394,8 +6429,8 @@
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="3" t="str">
-        <f>B12</f>
+      <c r="C20" s="3" t="str">
+        <f>C12</f>
         <v>2b7e151628aed2a6abf7158809cf4f3c</v>
       </c>
       <c r="G20" s="2"/>
@@ -6404,8 +6439,8 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="str">
-        <f>B14</f>
+      <c r="C21" s="3" t="str">
+        <f>C14</f>
         <v>000102030405060708090A0B0C0D0E0F</v>
       </c>
       <c r="G21" s="2"/>
@@ -6414,8 +6449,12 @@
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3" t="str" cm="1">
-        <f t="array" ref="B22">AES_Encrypt(B20,B19,B18,B20)</f>
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22">Util_showFormula(C22)</f>
+        <v>=AES_Encrypt(C20,C19,C18,C20)</v>
+      </c>
+      <c r="C22" s="3" t="str" cm="1">
+        <f t="array" ref="C22">AES_Encrypt(C20,C19,C18,C20)</f>
         <v>3AD77BB40D7A3660A89ECAF32466EF97A254BE88E037DDD9D79FB6411C3F9DF8</v>
       </c>
       <c r="G22" s="2"/>
@@ -6424,8 +6463,12 @@
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="3" t="str" cm="1">
-        <f t="array" ref="B23">AES_Decrypt(B20,B22,B18,B21)</f>
+      <c r="B23" t="str" cm="1">
+        <f t="array" ref="B23">Util_showFormula(C23)</f>
+        <v>=AES_Decrypt(C20,C22,C18,C21)</v>
+      </c>
+      <c r="C23" s="3" t="str" cm="1">
+        <f t="array" ref="C23">AES_Decrypt(C20,C22,C18,C21)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
       <c r="E23">
@@ -6441,7 +6484,7 @@
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="2"/>
@@ -6450,8 +6493,8 @@
       <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3" t="str">
-        <f>B19</f>
+      <c r="C26" s="3" t="str">
+        <f>C19</f>
         <v>6bc1bee22e409f96e93d7e117393172a</v>
       </c>
       <c r="G26" s="2"/>
@@ -6460,8 +6503,8 @@
       <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="3" t="str">
-        <f>B19</f>
+      <c r="C27" s="3" t="str">
+        <f>C19</f>
         <v>6bc1bee22e409f96e93d7e117393172a</v>
       </c>
       <c r="G27" s="1"/>
@@ -6470,8 +6513,8 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="3" t="str">
-        <f>B21</f>
+      <c r="C28" s="3" t="str">
+        <f>C21</f>
         <v>000102030405060708090A0B0C0D0E0F</v>
       </c>
       <c r="G28" s="2"/>
@@ -6480,8 +6523,12 @@
       <c r="A29" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="3" t="str" cm="1">
-        <f t="array" ref="B29">DES_Encrypt(B27,B26,B25,B27)</f>
+      <c r="B29" t="str" cm="1">
+        <f t="array" ref="B29">Util_showFormula(C29)</f>
+        <v>=DES_Encrypt(C27,C26,C25,C27)</v>
+      </c>
+      <c r="C29" s="3" t="str" cm="1">
+        <f t="array" ref="C29">DES_Encrypt(C27,C26,C25,C27)</f>
         <v>D83CC5F9634983CC8D92FF5B4A8DAD34E5DFE1913DC62854</v>
       </c>
     </row>
@@ -6489,61 +6536,74 @@
       <c r="A30" t="s">
         <v>233</v>
       </c>
-      <c r="B30" s="3" t="str" cm="1">
-        <f t="array" ref="B30">DES_decrypt(B27,B29,B25,B28)</f>
+      <c r="B30" t="str" cm="1">
+        <f t="array" ref="B30">Util_showFormula(C30)</f>
+        <v>=DES_decrypt(C27,C29,C25,C28)</v>
+      </c>
+      <c r="C30" s="3" t="str" cm="1">
+        <f t="array" ref="C30">DES_decrypt(C27,C29,C25,C28)</f>
         <v>6BC1BEE22E409F96E93D7E117393172A</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" t="s">
-        <v>325</v>
+      <c r="A32" t="s">
+        <v>576</v>
+      </c>
+      <c r="B32" t="str" cm="1">
+        <f t="array" ref="B32">Util_showFormula(C32)</f>
+        <v>=DES_KCV(C27)</v>
+      </c>
+      <c r="C32" t="str" cm="1">
+        <f t="array" ref="C32">DES_KCV(C27)</f>
+        <v>BA3093EF</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>279</v>
-      </c>
-      <c r="C33" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>569</v>
+        <v>578</v>
+      </c>
+      <c r="B33" t="str" cm="1">
+        <f t="array" ref="B33">Util_showFormula(C33)</f>
+        <v>=AES_KCV(C27)</v>
+      </c>
+      <c r="C33" t="str" cm="1">
+        <f t="array" ref="C33">AES_KCV(C27)</f>
+        <v>4411CAD8</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>325</v>
+        <v>577</v>
+      </c>
+      <c r="C35" t="str">
+        <f>"0000000000000000"</f>
+        <v>0000000000000000</v>
       </c>
       <c r="F35">
-        <f>LEN(C36)</f>
+        <f>LEN(C45)</f>
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>570</v>
-      </c>
-      <c r="C36" t="s">
-        <v>573</v>
+      <c r="B36" t="str" cm="1">
+        <f t="array" ref="B36">Util_showFormula(C36)</f>
+        <v>=DES_Encrypt(C27,C35,"ECB",C35)</v>
+      </c>
+      <c r="C36" t="str" cm="1">
+        <f t="array" ref="C36">DES_Encrypt(C27,C35,"ECB",C35)</f>
+        <v>BA3093EFA0671876E5DFE1913DC62854</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>571</v>
-      </c>
-      <c r="C37">
-        <v>16</v>
+        <v>579</v>
+      </c>
+      <c r="C37" t="str">
+        <f>C35&amp;C35</f>
+        <v>00000000000000000000000000000000</v>
       </c>
       <c r="E37">
-        <f>LEN(C38)</f>
+        <f>LEN(C47)</f>
         <v>104</v>
       </c>
       <c r="H37">
@@ -6551,26 +6611,81 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" t="s">
+      <c r="B38" t="str" cm="1">
+        <f t="array" ref="B38">Util_showFormula(C38)</f>
+        <v>=AES_Encrypt(C27,C37,"ECB",C37)</v>
+      </c>
+      <c r="C38" t="str" cm="1">
+        <f t="array" ref="C38">AES_Encrypt(C27,C37,"ECB",C37)</f>
+        <v>4411CAD8B52BE04A57891FF70D8F3A0BC81AB2EA9BABA40E94AF22B0C117F5F7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>279</v>
+      </c>
+      <c r="C42" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>570</v>
+      </c>
+      <c r="C45" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>571</v>
+      </c>
+      <c r="C46">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
         <v>438</v>
       </c>
-      <c r="C38" t="str" cm="1">
-        <f t="array" ref="C38">AES_Encrypt(C33,C34,C35,C36,C37)</f>
+      <c r="C47" t="str" cm="1">
+        <f t="array" ref="C47">AES_Encrypt(C42,C43,C44,C45,C46)</f>
         <v>0E3FF3977F23489D4D320C8303F11E8A559ED3E16E5648E3049AC65A876E64A7A77C3C643737EBE03DD4BE8A901274F3C6F2D949</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="C39" t="str" cm="1">
-        <f t="array" ref="C39">AES_Decrypt(C33,C38,C35,C36,C37)</f>
+      <c r="C48" t="str" cm="1">
+        <f t="array" ref="C48">AES_Decrypt(C42,C47,C44,C45,C46)</f>
         <v>486920416C69636520776861742061626F75742064696E6E657220746F6E69676874203F</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="C41" t="str" cm="1">
-        <f t="array" ref="C41">Util_HexStrToBase64(C38)</f>
+    <row r="50" spans="3:3">
+      <c r="C50" t="str" cm="1">
+        <f t="array" ref="C50">Util_HexStrToBase64(C47)</f>
         <v>Dj/zl38jSJ1NMgyDA/EeilWe0+FuVkjjBJrGWoduZKenfDxkNzfr4D3UvoqQEnTz_x000D_
 xvLZSQ==</v>
       </c>
@@ -6646,7 +6761,7 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">RSA_Encrypt(C1,C3)</f>
-        <v>4A3010F111BFDDC8A4BE776DCE44C215B53E56DA935DDB6FE05D0470A6C8CD1FA6DAB0304671489E2ADF7FBF476F06B8B801C20D4307E95F4FE2F3C4E00B81737C6DBC76A152C610B706785F6DFDDCDBEC47671A83B4294D5FB7C2ACAD11E94FBF676FA9329658FCEA6C83A55756A74110FAE397D5BC0713431442D454B94D9608A1841D0A500D63B8C6F714ED86D9431432D01E534BC5E5DC176D51834CB24D8500485A3C539919A20A02C0EC1AB5E2A3292010F05F12B693516486938D4A84FC9A1B89B6B6D47C8756219F92C8E41392E7B9A021A629BF407F28AE6FACAB6957C02A6ED7BAE7618FA16BB2C70427741CC7881DEE26BF03665631FB33C6F67A</v>
+        <v>30DAC329B0DF88EC00F451E4833F9349BD6EAA04AFE639E660EBB69B5D0A7218731C834813E8863D5BB148972CF2DEF1FF5D638DAC1FC92977082ED1354611BA352024C02E3499B6B4804390CA55F6CBF377C23EAA14ABD1E8B2F99B6C6F5BAE453F2D049FE99B6E6FD9C6BF5E2A6EA2AD66EEF68BC5C9FBFD3FE43C753691AD1D4EE14BF267A377A85EC2C00FC74926650B3D9CADA1C07C2FDB756E7D3ABA5F124EB99036E04CCA8BB2107D10E6D962FA11B8094E9B72EB76CC5A71DC80A95EBAC170A9E5B37F99E0CF9E3CE697EAFA2E29DD742ABF6A1AC4B1D4C34F6605E703E432AE74EB7068EB50A3CF19F5E7097EB1FDB2B9FAB1D2186B36210197A33F</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6751,7 +6866,7 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">RSA_Encrypt(C10,C3,C11,C12,C13)</f>
-        <v>436657D2D453D9C8ABFC48603789B0B399CAA9F3A1F2AFB5AFBA5435C1AEB3BD1FA7233FD62AD8E162065169433E35C5DF8D0104C9C2945B2F24D2B2B90206E4EE75B4B97B4ED0C696AD3DB5D34545A4FE026587EA5F440FE7895B6D5EAFACCADB8D28659F54BC1600CC8EBA436FA126A9A467983C4C971A19D0B8AD70E8DF6D709DDA097E5B9545E4650FCBF041D327E143549A6F81B6496B50B863C421B3AFEEEEB31FA688F956FEE42E3380DC8B0A8664426320364629EF308F8FE349898E1AB4932E3464C1F7D65277C98DCEEE59259AFFB59373250B1F8D76502F0B0F85CDF9F9A6153247EDA1A06FC02E6AE58F021420E8A509C36406ECB219C6CA1AD5</v>
+        <v>61BAB470DC93AF63558A9DC30BA33FFC84FBC4C736BA618AFDBF364D427CEF8D674F96F4B37A629E9AD9286E45F9E8C54D5C6F095B539EC06B804ADA0B0A635A1A2ECF5EF310180D56893B9A159BA0FAD2185843DA8D278438BBB3D3219DBD30C35552DD6CD2A506E7C31E7EEFEE8BB93C5F70AB67F62A311BE877FFF217A10A7803FDCF92C8198394D6B229ECACFCFDC2811ABED2FE392FEF7014DF97154AFD39675A018013C8ED69E0CC17B5B307B819376210DB7AF74F85F8CDDEA07F5D976F2750AC9A394F5BB144B735CA7ECA5BE4268AB453A5B070F6D7D1B9BD3AF0B7DB000214D6B98DA4CE2B0DC01A97D8CF9FC8EA43802A75D78EFD5D6EF277F2BC</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -6770,7 +6885,7 @@
     <row r="16" spans="1:3">
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">RSA_Encrypt(C1,C3,C11,C12,C13)</f>
-        <v>3D0FEB0195098E7AAA785E876A829CB252B41C7420A01CDD854CE99243ED29B57976820B47D14FD772545B2787B112AD858F5A1367F278FEF494837B8C0C106D7E03C9B8F4E86AF0DCBD4D7E5D9796F0EF3C7B93BFDB7105FDB4C55402341BAFB035A48B78BB94C34F1FFBADE35113B72AF6A45804B34142E2F1C56B8AEE6A32CE04EBFEA3E314BB179B46718D9BD69F3DA0B82E7DBFEBC8682237FF1318F2B15018468E7B0498F98456900558D5A8259A462FF077D45E131E4FF52419E509C7D526FE7E3D3D25A53E27BE5B1CE25170E9838B9826A08D25E3908ADB0DDD0F264B73E3002A90FA0DCC9781FBE8A17C7CB3B006F9AAAD177EDB5E02507678272A</v>
+        <v>0A175CEB8585A7388EAC9072D0F0308C038C18401ACDC319624FDE40C9A9B91A349F27B08BE545BB7C1CF34BE87879E841DF2A6ED737ED127A5CCEB6437F0BC1663FE8C489E32940FF702F239AFE64E69381A127FC171C0C6E431A98644FFC7926511A1AB1D0F88BD5154753B2CF4C146EC7A415B961CB347B732101B26348FFE10D364632A97E90E013F37AD37F96455DD51682407211F121BE4D7DF564DED754960F99855B2D065409071FF6203A7DD24A85234A19F9B75F1FD3485C0D0890D8F775CB3E6A514D0E9C04C673145D79F40E6B15E9D5F410F53E80153722269A1E08468A4D43B90120AA280E8054A2B9F1FC1F4894AFDD235FA8A15F848A450B</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6827,7 +6942,7 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">RSA_Encrypt(C1,C3,C19,C20,C21)</f>
-        <v>6FE6368E71211F5541440F4B40EA00B034130095A450DAD4A75A348DFB9185A677B77359022AECE9677B1346148064A3B9627B94FAA4E511CFEBB8FA9E463E39474B15D3719D6FB240AE569B6B70D9684C0C109A540D4A5FAA00AD45778715D368838ECE12E81791BD467E0A374C9B6D45FEB4C1A47D95F0BFDD26077AC469687F56CDE457AF23A4223EFBA94A0B43C48D302CF42A8F7767A2422EC26E16E8DB333329C4FE39710A00877741FD143216301BC0B98BBE8D332EC0FD1C4CEA06C5EEC670874CF0239D2360ECB5C2F0E27B4EF69B9D403209113F4F297C95291FD8F252E897923E8678B918905B4B014EB45C3248456AE991F68D30C05E3A6B8A6F</v>
+        <v>5ED0389281AB1A0EA153CE8611CD5236FA2352B4669966EBAD7F891FD656753ACEE0B9ABA74C347CA0188D50893D16B1BA344FC2751C11FF0F608E436A3C2924493324CEE033966D3205B12F46996C66DF75A8D8D09B6E6FDEDE7E353D0CD741785C486664B8FF3CEE835A09B9716E9C3695ED76F29827E2AB7F850C03796F3B98C0529695BD2EED96E64ACF3486BA41FCEFCBB3F26A458F9FB83860DA6C217241E6233A75785FDC549D9729496D7146989037C3E31379FFBBC422746895818809696CDB4CBC31DB5647546BB0FA516DE2EC9E91787B8C7E42D10DE8F38DCB23725E09A53A7E40B698115B4556668B1EA2DAFAACED5661C0FD622E058C8DE2F9</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -6853,12 +6968,12 @@
       </c>
       <c r="C26" t="str" cm="1">
         <f t="array" ref="C26">Util_HexStrToBase64(C22)</f>
-        <v>b+Y2jnEhH1VBRA9LQOoAsDQTAJWkUNrUp1o0jfuRhaZ3t3NZAirs6Wd7E0YUgGSj_x000D_
-uWJ7lPqk5RHP67j6nkY+OUdLFdNxnW+yQK5Wm2tw2WhMDBCaVA1KX6oArUV3hxXT_x000D_
-aIOOzhLoF5G9Rn4KN0ybbUX+tMGkfZXwv90mB3rEaWh/Vs3kV68jpCI++6lKC0PE_x000D_
-jTAs9CqPd2eiQi7Cbhbo2zMzKcT+OXEKAId3Qf0UMhYwG8C5i76NMy7A/RxM6gbF_x000D_
-7sZwh0zwI50jYOy1wvDie072m51AMgkRP08pfJUpH9jyUuiXkj6GeLkYkFtLAU60_x000D_
-XDJIRWrpkfaNMMBeOmuKbw==</v>
+        <v>XtA4koGrGg6hU86GEc1SNvojUrRmmWbrrX+JH9ZWdTrO4Lmrp0w0fKAYjVCJPRax_x000D_
+ujRPwnUcEf8PYI5DajwpJEkzJM7gM5ZtMgWxL0aZbGbfdajY0Jtub97efjU9DNdB_x000D_
+eFxIZmS4/zzug1oJuXFunDaV7XbymCfiq3+FDAN5bzuYwFKWlb0u7ZbmSs80hrpB_x000D_
+/O/Ls/JqRY+fuDhg2mwhckHmIzp1eF/cVJ2XKUltcUaYkDfD4xN5/7vEInRolYGI_x000D_
+CWls20y8MdtWR1RrsPpRbeLsnpF4e4x+QtEN6PONyyNyXgmlOn5AtpgRW0VWZose_x000D_
+otr6rO1WYcD9Yi4FjI3i+Q==</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -8243,7 +8358,7 @@
       </c>
       <c r="C67" t="str" cm="1">
         <f t="array" ref="C67">EC_SignHash(C64,C65,C66)</f>
-        <v>3046022100A6C41900021D0D90F72D731B09273A027400802480AD502CB870CB10EA4915D3022100EB1D2D79FD5A963773404BEC8A5615C7537A0D3D2174BF5348B8C336A721F673</v>
+        <v>304602210081C7D616366AFDCA6299749EC2015B6844EA7760B29712784ED9BF66BC340F86022100866F71E9955F7DE64045E1D129FF0CE0262F533094D1645640F4B8CCCA9847A8</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -8256,8 +8371,8 @@
       </c>
       <c r="C68" t="str" cm="1">
         <f t="array" ref="C68">Util_HexStrToBase64(C67)</f>
-        <v>MEYCIQCmxBkAAh0NkPctcxsJJzoCdACAJICtUCy4cMsQ6kkV0wIhAOsdLXn9WpY3_x000D_
-c0BL7IpWFcdTeg09IXS/U0i4wzanIfZz</v>
+        <v>MEYCIQCBx9YWNmr9ymKZdJ7CAVtoROp3YLKXEnhO2b9mvDQPhgIhAIZvcemVX33m_x000D_
+QEXh0Sn/DOAmL1MwlNFkVkD0uMzKmEeo</v>
       </c>
     </row>
     <row r="69" spans="1:3">

</xml_diff>